<commit_message>
currencies now works. (That was difficult.)
</commit_message>
<xml_diff>
--- a/www/countries.xlsx
+++ b/www/countries.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24611"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="151" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F52B8CB-F447-483B-B285-B169EAF80DBD}"/>
+  <xr:revisionPtr revIDLastSave="159" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C30B0C6-369A-48A4-B5E2-B87E0532CCD1}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="32">
   <si>
     <t>country</t>
   </si>
@@ -101,13 +101,16 @@
     <t>symbol</t>
   </si>
   <si>
-    <t>currency</t>
+    <t>currency_icon</t>
+  </si>
+  <si>
+    <t>currency_text</t>
   </si>
   <si>
     <t>cn</t>
   </si>
   <si>
-    <t>icon("yen")</t>
+    <t>yen</t>
   </si>
   <si>
     <t>vn</t>
@@ -119,7 +122,7 @@
     <t>kh</t>
   </si>
   <si>
-    <t>KH</t>
+    <t>KHR</t>
   </si>
 </sst>
 </file>
@@ -1093,18 +1096,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65B9C1BB-7C40-4454-AEC4-706923C51507}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:C1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1114,38 +1118,41 @@
       <c r="C1" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" t="s">
         <v>30</v>
+      </c>
+      <c r="D4" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sort of fixed currencies
</commit_message>
<xml_diff>
--- a/www/countries.xlsx
+++ b/www/countries.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thister\3D Objects\misc\GFP\www\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/64e43aabd8ba585a/Documents/GFP/www/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D0553DD-8982-4BBE-9A71-8A67389F04CD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{1D0553DD-8982-4BBE-9A71-8A67389F04CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{600BE43D-B5C2-49BE-9E8E-48A70AD1F1A0}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="defaults" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="36">
   <si>
     <t>country</t>
   </si>
@@ -94,9 +94,6 @@
     <t>Cambodia</t>
   </si>
   <si>
-    <t>symbol</t>
-  </si>
-  <si>
     <t>currency_icon</t>
   </si>
   <si>
@@ -131,6 +128,21 @@
   </si>
   <si>
     <t>new_hens</t>
+  </si>
+  <si>
+    <t>flag_symbol</t>
+  </si>
+  <si>
+    <t>CNY</t>
+  </si>
+  <si>
+    <t>locale</t>
+  </si>
+  <si>
+    <t>zh-CN</t>
+  </si>
+  <si>
+    <t>vi-VN</t>
   </si>
 </sst>
 </file>
@@ -494,7 +506,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -848,7 +860,7 @@
         <v>18</v>
       </c>
       <c r="B32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C32" s="1">
         <v>14</v>
@@ -859,7 +871,7 @@
         <v>3</v>
       </c>
       <c r="B33" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C33" s="1">
         <v>14</v>
@@ -870,7 +882,7 @@
         <v>17</v>
       </c>
       <c r="B34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C34" s="1">
         <v>15</v>
@@ -916,7 +928,7 @@
         <v>18</v>
       </c>
       <c r="B38" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C38" s="1">
         <v>2</v>
@@ -928,7 +940,7 @@
         <v>3</v>
       </c>
       <c r="B39" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C39" s="1">
         <v>2</v>
@@ -940,7 +952,7 @@
         <v>17</v>
       </c>
       <c r="B40" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C40" s="1">
         <v>2</v>
@@ -988,7 +1000,7 @@
         <v>18</v>
       </c>
       <c r="B44" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C44" s="1">
         <v>500</v>
@@ -1000,7 +1012,7 @@
         <v>3</v>
       </c>
       <c r="B45" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C45" s="1">
         <v>500</v>
@@ -1012,7 +1024,7 @@
         <v>17</v>
       </c>
       <c r="B46" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C46" s="1">
         <v>600</v>
@@ -1060,7 +1072,7 @@
         <v>18</v>
       </c>
       <c r="B50" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C50" s="1">
         <v>5000</v>
@@ -1072,7 +1084,7 @@
         <v>3</v>
       </c>
       <c r="B51" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C51" s="1">
         <v>5000</v>
@@ -1084,7 +1096,7 @@
         <v>17</v>
       </c>
       <c r="B52" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C52" s="1">
         <v>5000</v>
@@ -1102,66 +1114,81 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65B9C1BB-7C40-4454-AEC4-706923C51507}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>24</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>26</v>
-      </c>
-      <c r="D4" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed lots of things such as the countries.xlsx spreadsheet and the handling of currencies. probably other stuff too.
</commit_message>
<xml_diff>
--- a/www/countries.xlsx
+++ b/www/countries.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/64e43aabd8ba585a/Documents/GFP/www/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{1D0553DD-8982-4BBE-9A71-8A67389F04CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{600BE43D-B5C2-49BE-9E8E-48A70AD1F1A0}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{6045025C-A6C3-4296-9907-33F4F2624F88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB216A8E-FE44-4C77-B5A7-E11C885BD662}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="defaults" sheetId="1" r:id="rId1"/>
-    <sheet name="countries" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
+    <sheet name="defaults" sheetId="1" r:id="rId2"/>
+    <sheet name="countries" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">defaults!$A$1:$C$49</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">defaults!$A$1:$C$49</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="42">
   <si>
     <t>country</t>
   </si>
@@ -143,6 +144,24 @@
   </si>
   <si>
     <t>vi-VN</t>
+  </si>
+  <si>
+    <t>lay_percent</t>
+  </si>
+  <si>
+    <t>currency_unicode</t>
+  </si>
+  <si>
+    <t>currency_locale</t>
+  </si>
+  <si>
+    <t>\U20AB</t>
+  </si>
+  <si>
+    <t>\U00A5</t>
+  </si>
+  <si>
+    <t>\U17DB</t>
   </si>
 </sst>
 </file>
@@ -503,10 +522,326 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F017957-BA31-4BBB-B7FE-43888E5CFB3F}">
+  <dimension ref="A1:V4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="R1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="V3" sqref="V3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2">
+        <v>5001</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1">
+        <v>5000</v>
+      </c>
+      <c r="G2" s="1">
+        <v>4</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="I2" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="K2" s="1">
+        <v>500</v>
+      </c>
+      <c r="L2">
+        <v>801</v>
+      </c>
+      <c r="M2">
+        <v>2.8</v>
+      </c>
+      <c r="N2">
+        <v>1.4</v>
+      </c>
+      <c r="O2">
+        <v>2.1</v>
+      </c>
+      <c r="P2">
+        <v>1.9</v>
+      </c>
+      <c r="Q2">
+        <v>40001</v>
+      </c>
+      <c r="R2">
+        <v>50001</v>
+      </c>
+      <c r="S2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T2" t="s">
+        <v>26</v>
+      </c>
+      <c r="U2" t="s">
+        <v>35</v>
+      </c>
+      <c r="V2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>10000</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1">
+        <v>5000</v>
+      </c>
+      <c r="G3" s="1">
+        <v>2</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0.98</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0.53</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="K3" s="1">
+        <v>500</v>
+      </c>
+      <c r="L3">
+        <v>1000</v>
+      </c>
+      <c r="M3">
+        <v>1.2</v>
+      </c>
+      <c r="N3">
+        <v>3</v>
+      </c>
+      <c r="O3">
+        <v>2</v>
+      </c>
+      <c r="P3">
+        <v>3</v>
+      </c>
+      <c r="Q3">
+        <v>30000</v>
+      </c>
+      <c r="R3">
+        <v>34000</v>
+      </c>
+      <c r="S3" t="s">
+        <v>21</v>
+      </c>
+      <c r="T3" t="s">
+        <v>32</v>
+      </c>
+      <c r="U3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4">
+        <v>5000</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2</v>
+      </c>
+      <c r="F4" s="1">
+        <v>5000</v>
+      </c>
+      <c r="G4" s="1">
+        <v>3</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.97</v>
+      </c>
+      <c r="I4" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0.09</v>
+      </c>
+      <c r="K4" s="1">
+        <v>600</v>
+      </c>
+      <c r="L4">
+        <v>800</v>
+      </c>
+      <c r="M4">
+        <v>1.8</v>
+      </c>
+      <c r="N4">
+        <v>0.4</v>
+      </c>
+      <c r="O4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P4">
+        <v>0.9</v>
+      </c>
+      <c r="Q4">
+        <v>40000</v>
+      </c>
+      <c r="R4">
+        <v>50000</v>
+      </c>
+      <c r="S4" t="s">
+        <v>23</v>
+      </c>
+      <c r="T4" t="s">
+        <v>24</v>
+      </c>
+      <c r="U4" t="s">
+        <v>35</v>
+      </c>
+      <c r="V4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:BF55"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -514,7 +849,7 @@
     <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -525,7 +860,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -536,7 +871,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -547,7 +882,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -557,8 +892,35 @@
       <c r="C4" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="AI4" s="1"/>
+      <c r="AJ4" s="1"/>
+      <c r="AK4" s="1"/>
+      <c r="AL4" s="1"/>
+      <c r="AM4" s="1"/>
+      <c r="AN4" s="1"/>
+      <c r="AO4" s="1"/>
+      <c r="AP4" s="1"/>
+      <c r="AQ4" s="1"/>
+      <c r="AR4" s="1"/>
+      <c r="AS4" s="1"/>
+      <c r="AT4" s="1"/>
+      <c r="AU4" s="1"/>
+      <c r="AV4" s="1"/>
+      <c r="AW4" s="1"/>
+      <c r="AX4" s="1"/>
+      <c r="AY4" s="1"/>
+      <c r="AZ4" s="1"/>
+      <c r="BA4" s="1"/>
+      <c r="BB4" s="1"/>
+      <c r="BC4" s="1"/>
+      <c r="BD4" s="1"/>
+      <c r="BE4" s="1"/>
+      <c r="BF4" s="1"/>
+    </row>
+    <row r="5" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -569,7 +931,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -580,7 +942,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -591,7 +953,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -602,7 +964,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -613,7 +975,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -624,7 +986,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -635,7 +997,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -646,7 +1008,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -657,7 +1019,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -668,7 +1030,7 @@
         <v>40001</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -679,7 +1041,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1102,6 +1464,39 @@
         <v>5000</v>
       </c>
       <c r="D52" s="1"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>18</v>
+      </c>
+      <c r="B53" t="s">
+        <v>36</v>
+      </c>
+      <c r="C53" s="1">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>3</v>
+      </c>
+      <c r="B54" t="s">
+        <v>36</v>
+      </c>
+      <c r="C54" s="1">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>17</v>
+      </c>
+      <c r="B55" t="s">
+        <v>36</v>
+      </c>
+      <c r="C55" s="1">
+        <v>0.97</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C49">
@@ -1112,12 +1507,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65B9C1BB-7C40-4454-AEC4-706923C51507}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added some currencies to the spreadsheet
</commit_message>
<xml_diff>
--- a/www/countries.xlsx
+++ b/www/countries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thister\3D Objects\misc\GFP\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0354EFF-7E15-4E45-B4EC-A694672657B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A9AC10-70A1-4A67-A4E6-8FB08CF54418}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,6 +34,9 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={F72E4B61-D5B3-4232-A273-C5B8148054DB}</author>
+    <author>tc={913484B7-6738-4C0B-9D52-5C5B580E52D3}</author>
+    <author>tc={B52CFFF6-B892-4A1F-92BB-FA3C18ABD93E}</author>
+    <author>tc={E851F89F-495A-4D89-9F0E-B346D8426901}</author>
   </authors>
   <commentList>
     <comment ref="A21" authorId="0" shapeId="0" xr:uid="{F72E4B61-D5B3-4232-A273-C5B8148054DB}">
@@ -44,12 +47,36 @@
     https://cdn.jsdelivr.net/gh/lipis/flag-icon-css@master/flags/4x3/</t>
       </text>
     </comment>
+    <comment ref="A23" authorId="1" shapeId="0" xr:uid="{913484B7-6738-4C0B-9D52-5C5B580E52D3}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    https://docs.microsoft.com/en-us/openspecs/office_standards/ms-oe376/6c085406-a698-4e12-9d4d-c3b0ee3dbc4a</t>
+      </text>
+    </comment>
+    <comment ref="A24" authorId="2" shapeId="0" xr:uid="{B52CFFF6-B892-4A1F-92BB-FA3C18ABD93E}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    https://www.compart.com/en/unicode/category/Sc</t>
+      </text>
+    </comment>
+    <comment ref="A25" authorId="3" shapeId="0" xr:uid="{E851F89F-495A-4D89-9F0E-B346D8426901}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    https://en.wikipedia.org/wiki/Currency_symbol</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="93">
   <si>
     <t>country</t>
   </si>
@@ -271,6 +298,63 @@
   </si>
   <si>
     <t>us</t>
+  </si>
+  <si>
+    <t>IDR</t>
+  </si>
+  <si>
+    <t>THB</t>
+  </si>
+  <si>
+    <t>JPY</t>
+  </si>
+  <si>
+    <t>RM</t>
+  </si>
+  <si>
+    <t>SGD</t>
+  </si>
+  <si>
+    <t>KRW</t>
+  </si>
+  <si>
+    <t>PHP</t>
+  </si>
+  <si>
+    <t>\U0E3F</t>
+  </si>
+  <si>
+    <t>Rp</t>
+  </si>
+  <si>
+    <t>S$</t>
+  </si>
+  <si>
+    <t>₩</t>
+  </si>
+  <si>
+    <t>₱</t>
+  </si>
+  <si>
+    <t>¥</t>
+  </si>
+  <si>
+    <t>฿</t>
+  </si>
+  <si>
+    <t>currency_symbol</t>
+  </si>
+  <si>
+    <t>\U20B1</t>
+  </si>
+  <si>
+    <t>$</t>
+  </si>
+  <si>
+    <t>៛</t>
+  </si>
+  <si>
+    <t>₫</t>
   </si>
 </sst>
 </file>
@@ -311,7 +395,7 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -664,15 +748,24 @@
   <threadedComment ref="A21" dT="2022-01-14T23:37:47.93" personId="{68507162-D81B-4C03-812D-5D852E98FF85}" id="{F72E4B61-D5B3-4232-A273-C5B8148054DB}">
     <text>https://cdn.jsdelivr.net/gh/lipis/flag-icon-css@master/flags/4x3/</text>
   </threadedComment>
+  <threadedComment ref="A23" dT="2022-01-18T21:56:41.13" personId="{68507162-D81B-4C03-812D-5D852E98FF85}" id="{913484B7-6738-4C0B-9D52-5C5B580E52D3}">
+    <text>https://docs.microsoft.com/en-us/openspecs/office_standards/ms-oe376/6c085406-a698-4e12-9d4d-c3b0ee3dbc4a</text>
+  </threadedComment>
+  <threadedComment ref="A24" dT="2022-01-18T21:09:38.62" personId="{68507162-D81B-4C03-812D-5D852E98FF85}" id="{B52CFFF6-B892-4A1F-92BB-FA3C18ABD93E}">
+    <text>https://www.compart.com/en/unicode/category/Sc</text>
+  </threadedComment>
+  <threadedComment ref="A25" dT="2022-01-18T21:18:28.00" personId="{68507162-D81B-4C03-812D-5D852E98FF85}" id="{E851F89F-495A-4D89-9F0E-B346D8426901}">
+    <text>https://en.wikipedia.org/wiki/Currency_symbol</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEED9D62-A800-438E-BFB7-65A02D07097D}">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -681,7 +774,7 @@
     <col min="2" max="2" width="7.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
@@ -1557,6 +1650,27 @@
       <c r="B22" t="s">
         <v>25</v>
       </c>
+      <c r="C22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D22" t="s">
+        <v>75</v>
+      </c>
+      <c r="E22" t="s">
+        <v>76</v>
+      </c>
+      <c r="F22" t="s">
+        <v>77</v>
+      </c>
+      <c r="G22" t="s">
+        <v>78</v>
+      </c>
+      <c r="H22" t="s">
+        <v>79</v>
+      </c>
+      <c r="I22" t="s">
+        <v>80</v>
+      </c>
       <c r="J22" t="s">
         <v>20</v>
       </c>
@@ -1585,11 +1699,61 @@
       <c r="B24" t="s">
         <v>32</v>
       </c>
+      <c r="C24" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" t="s">
+        <v>81</v>
+      </c>
+      <c r="E24" t="s">
+        <v>32</v>
+      </c>
+      <c r="I24" t="s">
+        <v>89</v>
+      </c>
       <c r="J24" t="s">
         <v>33</v>
       </c>
       <c r="K24" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B25" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25" t="s">
+        <v>87</v>
+      </c>
+      <c r="E25" t="s">
+        <v>86</v>
+      </c>
+      <c r="F25" t="s">
+        <v>77</v>
+      </c>
+      <c r="G25" t="s">
+        <v>83</v>
+      </c>
+      <c r="H25" t="s">
+        <v>84</v>
+      </c>
+      <c r="I25" t="s">
+        <v>85</v>
+      </c>
+      <c r="J25" t="s">
+        <v>91</v>
+      </c>
+      <c r="K25" t="s">
+        <v>92</v>
+      </c>
+      <c r="L25" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
small tweaks - it works - gonna send
</commit_message>
<xml_diff>
--- a/www/countries.xlsx
+++ b/www/countries.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thister\3D Objects\misc\GFP\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD94C781-1913-4786-96F7-326C419A15D9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A90C159-C815-4EE6-BE7D-D1E414CFA4A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="4" r:id="rId1"/>
@@ -34,8 +34,8 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={F72E4B61-D5B3-4232-A273-C5B8148054DB}</author>
+    <author>tc={87853F49-BFA8-4099-81C8-0A9DFBA77DAA}</author>
     <author>tc={913484B7-6738-4C0B-9D52-5C5B580E52D3}</author>
-    <author>tc={B52CFFF6-B892-4A1F-92BB-FA3C18ABD93E}</author>
     <author>tc={E851F89F-495A-4D89-9F0E-B346D8426901}</author>
   </authors>
   <commentList>
@@ -47,7 +47,15 @@
     https://cdn.jsdelivr.net/gh/lipis/flag-icon-css@master/flags/4x3/</t>
       </text>
     </comment>
-    <comment ref="A23" authorId="1" shapeId="0" xr:uid="{913484B7-6738-4C0B-9D52-5C5B580E52D3}">
+    <comment ref="A22" authorId="1" shapeId="0" xr:uid="{87853F49-BFA8-4099-81C8-0A9DFBA77DAA}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    https://en.wikipedia.org/wiki/Currency#Modern_currencies</t>
+      </text>
+    </comment>
+    <comment ref="A23" authorId="2" shapeId="0" xr:uid="{913484B7-6738-4C0B-9D52-5C5B580E52D3}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -55,15 +63,7 @@
     https://docs.microsoft.com/en-us/openspecs/office_standards/ms-oe376/6c085406-a698-4e12-9d4d-c3b0ee3dbc4a</t>
       </text>
     </comment>
-    <comment ref="A24" authorId="2" shapeId="0" xr:uid="{B52CFFF6-B892-4A1F-92BB-FA3C18ABD93E}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    https://www.compart.com/en/unicode/category/Sc</t>
-      </text>
-    </comment>
-    <comment ref="A25" authorId="3" shapeId="0" xr:uid="{E851F89F-495A-4D89-9F0E-B346D8426901}">
+    <comment ref="A24" authorId="3" shapeId="0" xr:uid="{E851F89F-495A-4D89-9F0E-B346D8426901}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="97">
   <si>
     <t>country</t>
   </si>
@@ -165,21 +165,9 @@
     <t>lay_percent</t>
   </si>
   <si>
-    <t>currency_unicode</t>
-  </si>
-  <si>
     <t>currency_locale</t>
   </si>
   <si>
-    <t>\U20AB</t>
-  </si>
-  <si>
-    <t>\U00A5</t>
-  </si>
-  <si>
-    <t>\U17DB</t>
-  </si>
-  <si>
     <t>blurb</t>
   </si>
   <si>
@@ -321,9 +309,6 @@
     <t>PHP</t>
   </si>
   <si>
-    <t>\U0E3F</t>
-  </si>
-  <si>
     <t>Rp</t>
   </si>
   <si>
@@ -345,9 +330,6 @@
     <t>currency_symbol</t>
   </si>
   <si>
-    <t>\U20B1</t>
-  </si>
-  <si>
     <t>$</t>
   </si>
   <si>
@@ -366,20 +348,32 @@
     <t>ja-JP</t>
   </si>
   <si>
-    <t>ms-MY</t>
-  </si>
-  <si>
     <t>th-TH</t>
   </si>
   <si>
     <t>USD</t>
+  </si>
+  <si>
+    <t>zh-SG</t>
+  </si>
+  <si>
+    <t>en-PH</t>
+  </si>
+  <si>
+    <t>id-ID</t>
+  </si>
+  <si>
+    <t>en-MY</t>
+  </si>
+  <si>
+    <t>MYR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -408,6 +402,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -760,13 +760,13 @@
   <threadedComment ref="A21" dT="2022-01-14T23:37:47.93" personId="{68507162-D81B-4C03-812D-5D852E98FF85}" id="{F72E4B61-D5B3-4232-A273-C5B8148054DB}">
     <text>https://cdn.jsdelivr.net/gh/lipis/flag-icon-css@master/flags/4x3/</text>
   </threadedComment>
+  <threadedComment ref="A22" dT="2022-01-19T21:35:23.09" personId="{68507162-D81B-4C03-812D-5D852E98FF85}" id="{87853F49-BFA8-4099-81C8-0A9DFBA77DAA}">
+    <text>https://en.wikipedia.org/wiki/Currency#Modern_currencies</text>
+  </threadedComment>
   <threadedComment ref="A23" dT="2022-01-18T21:56:41.13" personId="{68507162-D81B-4C03-812D-5D852E98FF85}" id="{913484B7-6738-4C0B-9D52-5C5B580E52D3}">
     <text>https://docs.microsoft.com/en-us/openspecs/office_standards/ms-oe376/6c085406-a698-4e12-9d4d-c3b0ee3dbc4a</text>
   </threadedComment>
-  <threadedComment ref="A24" dT="2022-01-18T21:09:38.62" personId="{68507162-D81B-4C03-812D-5D852E98FF85}" id="{B52CFFF6-B892-4A1F-92BB-FA3C18ABD93E}">
-    <text>https://www.compart.com/en/unicode/category/Sc</text>
-  </threadedComment>
-  <threadedComment ref="A25" dT="2022-01-18T21:18:28.00" personId="{68507162-D81B-4C03-812D-5D852E98FF85}" id="{E851F89F-495A-4D89-9F0E-B346D8426901}">
+  <threadedComment ref="A24" dT="2022-01-18T21:18:28.00" personId="{68507162-D81B-4C03-812D-5D852E98FF85}" id="{E851F89F-495A-4D89-9F0E-B346D8426901}">
     <text>https://en.wikipedia.org/wiki/Currency_symbol</text>
   </threadedComment>
 </ThreadedComments>
@@ -774,30 +774,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEED9D62-A800-438E-BFB7-65A02D07097D}">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.109375" customWidth="1"/>
-    <col min="13" max="13" width="92.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="102.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -805,25 +805,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>14</v>
@@ -832,13 +832,13 @@
         <v>13</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -876,10 +876,10 @@
         <v>0</v>
       </c>
       <c r="M2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -917,10 +917,10 @@
         <v>0</v>
       </c>
       <c r="M3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -958,10 +958,10 @@
         <v>0</v>
       </c>
       <c r="M4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>28</v>
       </c>
@@ -999,10 +999,10 @@
         <v>0</v>
       </c>
       <c r="M5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -1040,10 +1040,10 @@
         <v>0</v>
       </c>
       <c r="M6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -1081,10 +1081,10 @@
         <v>0</v>
       </c>
       <c r="M7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -1122,10 +1122,10 @@
         <v>0</v>
       </c>
       <c r="M8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -1163,10 +1163,10 @@
         <v>0</v>
       </c>
       <c r="M9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
@@ -1204,10 +1204,10 @@
         <v>0</v>
       </c>
       <c r="M10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
@@ -1245,10 +1245,10 @@
         <v>0</v>
       </c>
       <c r="M11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
@@ -1286,10 +1286,10 @@
         <v>0</v>
       </c>
       <c r="M12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
@@ -1327,10 +1327,10 @@
         <v>0</v>
       </c>
       <c r="M13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
@@ -1368,10 +1368,10 @@
         <v>0</v>
       </c>
       <c r="M14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -1409,10 +1409,10 @@
         <v>0</v>
       </c>
       <c r="M15" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
@@ -1450,136 +1450,136 @@
         <v>0</v>
       </c>
       <c r="M16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
-      <c r="M17" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="J18">
-        <v>0</v>
-      </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-      <c r="M18" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-      <c r="J19">
-        <v>0</v>
-      </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
-      <c r="M19" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="B20">
         <v>0</v>
       </c>
@@ -1614,10 +1614,10 @@
         <v>0</v>
       </c>
       <c r="M20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
@@ -1625,25 +1625,25 @@
         <v>16</v>
       </c>
       <c r="C21" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" t="s">
+        <v>63</v>
+      </c>
+      <c r="E21" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21" t="s">
+        <v>65</v>
+      </c>
+      <c r="G21" t="s">
         <v>66</v>
       </c>
-      <c r="D21" t="s">
+      <c r="H21" t="s">
         <v>67</v>
       </c>
-      <c r="E21" t="s">
+      <c r="I21" t="s">
         <v>68</v>
-      </c>
-      <c r="F21" t="s">
-        <v>69</v>
-      </c>
-      <c r="G21" t="s">
-        <v>70</v>
-      </c>
-      <c r="H21" t="s">
-        <v>71</v>
-      </c>
-      <c r="I21" t="s">
-        <v>72</v>
       </c>
       <c r="J21" t="s">
         <v>19</v>
@@ -1652,10 +1652,10 @@
         <v>17</v>
       </c>
       <c r="L21" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>15</v>
       </c>
@@ -1663,25 +1663,25 @@
         <v>25</v>
       </c>
       <c r="C22" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" t="s">
+        <v>72</v>
+      </c>
+      <c r="F22" t="s">
+        <v>96</v>
+      </c>
+      <c r="G22" t="s">
         <v>74</v>
       </c>
-      <c r="D22" t="s">
+      <c r="H22" t="s">
         <v>75</v>
       </c>
-      <c r="E22" t="s">
+      <c r="I22" t="s">
         <v>76</v>
-      </c>
-      <c r="F22" t="s">
-        <v>77</v>
-      </c>
-      <c r="G22" t="s">
-        <v>78</v>
-      </c>
-      <c r="H22" t="s">
-        <v>79</v>
-      </c>
-      <c r="I22" t="s">
-        <v>80</v>
       </c>
       <c r="J22" t="s">
         <v>20</v>
@@ -1690,27 +1690,36 @@
         <v>18</v>
       </c>
       <c r="L22" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" t="s">
         <v>26</v>
       </c>
+      <c r="C23" t="s">
+        <v>94</v>
+      </c>
       <c r="D23" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="E23" t="s">
+        <v>89</v>
+      </c>
+      <c r="F23" t="s">
         <v>95</v>
       </c>
-      <c r="F23" t="s">
-        <v>96</v>
+      <c r="G23" t="s">
+        <v>92</v>
       </c>
       <c r="H23" t="s">
-        <v>94</v>
+        <v>88</v>
+      </c>
+      <c r="I23" t="s">
+        <v>93</v>
       </c>
       <c r="J23" t="s">
         <v>27</v>
@@ -1719,71 +1728,45 @@
         <v>27</v>
       </c>
       <c r="L23" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>29</v>
+        <v>83</v>
       </c>
       <c r="B24" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="C24" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" t="s">
         <v>82</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>81</v>
       </c>
-      <c r="E24" t="s">
-        <v>32</v>
+      <c r="F24" t="s">
+        <v>73</v>
+      </c>
+      <c r="G24" t="s">
+        <v>78</v>
+      </c>
+      <c r="H24" t="s">
+        <v>79</v>
       </c>
       <c r="I24" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="J24" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="K24" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B25" t="s">
         <v>86</v>
       </c>
-      <c r="C25" t="s">
-        <v>82</v>
-      </c>
-      <c r="D25" t="s">
-        <v>87</v>
-      </c>
-      <c r="E25" t="s">
-        <v>86</v>
-      </c>
-      <c r="F25" t="s">
-        <v>77</v>
-      </c>
-      <c r="G25" t="s">
-        <v>83</v>
-      </c>
-      <c r="H25" t="s">
+      <c r="L24" t="s">
         <v>84</v>
-      </c>
-      <c r="I25" t="s">
-        <v>85</v>
-      </c>
-      <c r="J25" t="s">
-        <v>91</v>
-      </c>
-      <c r="K25" t="s">
-        <v>92</v>
-      </c>
-      <c r="L25" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
big fix on currencies
</commit_message>
<xml_diff>
--- a/www/countries.xlsx
+++ b/www/countries.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thister\3D Objects\misc\GFP\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A90C159-C815-4EE6-BE7D-D1E414CFA4A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3D556F9-4B0A-4411-92E0-B9B232B6D0D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="4" r:id="rId1"/>
@@ -34,9 +34,9 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={F72E4B61-D5B3-4232-A273-C5B8148054DB}</author>
-    <author>tc={87853F49-BFA8-4099-81C8-0A9DFBA77DAA}</author>
-    <author>tc={913484B7-6738-4C0B-9D52-5C5B580E52D3}</author>
     <author>tc={E851F89F-495A-4D89-9F0E-B346D8426901}</author>
+    <author>tc={93BA962B-F956-49AC-981E-211EFB48C9A2}</author>
+    <author>tc={E615448F-82C1-4B52-AAD0-13537DDB6395}</author>
   </authors>
   <commentList>
     <comment ref="A21" authorId="0" shapeId="0" xr:uid="{F72E4B61-D5B3-4232-A273-C5B8148054DB}">
@@ -47,23 +47,7 @@
     https://cdn.jsdelivr.net/gh/lipis/flag-icon-css@master/flags/4x3/</t>
       </text>
     </comment>
-    <comment ref="A22" authorId="1" shapeId="0" xr:uid="{87853F49-BFA8-4099-81C8-0A9DFBA77DAA}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    https://en.wikipedia.org/wiki/Currency#Modern_currencies</t>
-      </text>
-    </comment>
-    <comment ref="A23" authorId="2" shapeId="0" xr:uid="{913484B7-6738-4C0B-9D52-5C5B580E52D3}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    https://docs.microsoft.com/en-us/openspecs/office_standards/ms-oe376/6c085406-a698-4e12-9d4d-c3b0ee3dbc4a</t>
-      </text>
-    </comment>
-    <comment ref="A24" authorId="3" shapeId="0" xr:uid="{E851F89F-495A-4D89-9F0E-B346D8426901}">
+    <comment ref="A22" authorId="1" shapeId="0" xr:uid="{E851F89F-495A-4D89-9F0E-B346D8426901}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -71,12 +55,28 @@
     https://en.wikipedia.org/wiki/Currency_symbol</t>
       </text>
     </comment>
+    <comment ref="A23" authorId="2" shapeId="0" xr:uid="{93BA962B-F956-49AC-981E-211EFB48C9A2}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    put TRUE here if you want the currency symbol after the number</t>
+      </text>
+    </comment>
+    <comment ref="A24" authorId="3" shapeId="0" xr:uid="{E615448F-82C1-4B52-AAD0-13537DDB6395}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    put TRUE here if you want periods to separate thousands and a comma as the decimal symbol.</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="76">
   <si>
     <t>country</t>
   </si>
@@ -123,24 +123,15 @@
     <t>Cambodia</t>
   </si>
   <si>
-    <t>currency_text</t>
-  </si>
-  <si>
     <t>cn</t>
   </si>
   <si>
     <t>vn</t>
   </si>
   <si>
-    <t>VND</t>
-  </si>
-  <si>
     <t>kh</t>
   </si>
   <si>
-    <t>KHR</t>
-  </si>
-  <si>
     <t>period_length</t>
   </si>
   <si>
@@ -153,21 +144,9 @@
     <t>flag_symbol</t>
   </si>
   <si>
-    <t>CNY</t>
-  </si>
-  <si>
-    <t>zh-CN</t>
-  </si>
-  <si>
-    <t>vi-VN</t>
-  </si>
-  <si>
     <t>lay_percent</t>
   </si>
   <si>
-    <t>currency_locale</t>
-  </si>
-  <si>
     <t>blurb</t>
   </si>
   <si>
@@ -288,27 +267,9 @@
     <t>us</t>
   </si>
   <si>
-    <t>IDR</t>
-  </si>
-  <si>
-    <t>THB</t>
-  </si>
-  <si>
-    <t>JPY</t>
-  </si>
-  <si>
     <t>RM</t>
   </si>
   <si>
-    <t>SGD</t>
-  </si>
-  <si>
-    <t>KRW</t>
-  </si>
-  <si>
-    <t>PHP</t>
-  </si>
-  <si>
     <t>Rp</t>
   </si>
   <si>
@@ -339,34 +300,10 @@
     <t>₫</t>
   </si>
   <si>
-    <t>en-US</t>
-  </si>
-  <si>
-    <t>ko-KR</t>
-  </si>
-  <si>
-    <t>ja-JP</t>
-  </si>
-  <si>
-    <t>th-TH</t>
-  </si>
-  <si>
-    <t>USD</t>
-  </si>
-  <si>
-    <t>zh-SG</t>
-  </si>
-  <si>
-    <t>en-PH</t>
-  </si>
-  <si>
-    <t>id-ID</t>
-  </si>
-  <si>
-    <t>en-MY</t>
-  </si>
-  <si>
-    <t>MYR</t>
+    <t>suffix</t>
+  </si>
+  <si>
+    <t>reverse_marks</t>
   </si>
 </sst>
 </file>
@@ -407,7 +344,7 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -760,44 +697,44 @@
   <threadedComment ref="A21" dT="2022-01-14T23:37:47.93" personId="{68507162-D81B-4C03-812D-5D852E98FF85}" id="{F72E4B61-D5B3-4232-A273-C5B8148054DB}">
     <text>https://cdn.jsdelivr.net/gh/lipis/flag-icon-css@master/flags/4x3/</text>
   </threadedComment>
-  <threadedComment ref="A22" dT="2022-01-19T21:35:23.09" personId="{68507162-D81B-4C03-812D-5D852E98FF85}" id="{87853F49-BFA8-4099-81C8-0A9DFBA77DAA}">
-    <text>https://en.wikipedia.org/wiki/Currency#Modern_currencies</text>
+  <threadedComment ref="A22" dT="2022-01-18T21:18:28.00" personId="{68507162-D81B-4C03-812D-5D852E98FF85}" id="{E851F89F-495A-4D89-9F0E-B346D8426901}">
+    <text>https://en.wikipedia.org/wiki/Currency_symbol</text>
   </threadedComment>
-  <threadedComment ref="A23" dT="2022-01-18T21:56:41.13" personId="{68507162-D81B-4C03-812D-5D852E98FF85}" id="{913484B7-6738-4C0B-9D52-5C5B580E52D3}">
-    <text>https://docs.microsoft.com/en-us/openspecs/office_standards/ms-oe376/6c085406-a698-4e12-9d4d-c3b0ee3dbc4a</text>
+  <threadedComment ref="A23" dT="2022-03-23T23:17:12.92" personId="{68507162-D81B-4C03-812D-5D852E98FF85}" id="{93BA962B-F956-49AC-981E-211EFB48C9A2}">
+    <text>put TRUE here if you want the currency symbol after the number</text>
   </threadedComment>
-  <threadedComment ref="A24" dT="2022-01-18T21:18:28.00" personId="{68507162-D81B-4C03-812D-5D852E98FF85}" id="{E851F89F-495A-4D89-9F0E-B346D8426901}">
-    <text>https://en.wikipedia.org/wiki/Currency_symbol</text>
+  <threadedComment ref="A24" dT="2022-03-23T23:17:44.54" personId="{68507162-D81B-4C03-812D-5D852E98FF85}" id="{E615448F-82C1-4B52-AAD0-13537DDB6395}">
+    <text>put TRUE here if you want periods to separate thousands and a comma as the decimal symbol.</text>
   </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEED9D62-A800-438E-BFB7-65A02D07097D}">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="102.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="102.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -805,25 +742,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>14</v>
@@ -832,13 +769,13 @@
         <v>13</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -876,10 +813,10 @@
         <v>0</v>
       </c>
       <c r="M2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -917,12 +854,12 @@
         <v>0</v>
       </c>
       <c r="M3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -958,92 +895,92 @@
         <v>0</v>
       </c>
       <c r="M4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6" t="s">
         <v>28</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -1081,10 +1018,10 @@
         <v>0</v>
       </c>
       <c r="M7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -1122,10 +1059,10 @@
         <v>0</v>
       </c>
       <c r="M8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -1163,12 +1100,12 @@
         <v>0</v>
       </c>
       <c r="M9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -1204,10 +1141,10 @@
         <v>0</v>
       </c>
       <c r="M10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
@@ -1245,10 +1182,10 @@
         <v>0</v>
       </c>
       <c r="M11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
@@ -1286,10 +1223,10 @@
         <v>0</v>
       </c>
       <c r="M12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
@@ -1327,10 +1264,10 @@
         <v>0</v>
       </c>
       <c r="M13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
@@ -1368,10 +1305,10 @@
         <v>0</v>
       </c>
       <c r="M14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -1409,10 +1346,10 @@
         <v>0</v>
       </c>
       <c r="M15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
@@ -1450,95 +1387,95 @@
         <v>0</v>
       </c>
       <c r="M16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
-      <c r="M17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="J18">
-        <v>0</v>
-      </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-      <c r="M18" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="B19">
         <v>0</v>
       </c>
@@ -1573,13 +1510,13 @@
         <v>0</v>
       </c>
       <c r="M19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="B20">
         <v>0</v>
       </c>
@@ -1614,160 +1551,109 @@
         <v>0</v>
       </c>
       <c r="M20" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" t="s">
+        <v>57</v>
+      </c>
+      <c r="F21" t="s">
+        <v>58</v>
+      </c>
+      <c r="G21" t="s">
+        <v>59</v>
+      </c>
+      <c r="H21" t="s">
+        <v>60</v>
+      </c>
+      <c r="I21" t="s">
+        <v>61</v>
+      </c>
+      <c r="J21" t="s">
+        <v>17</v>
+      </c>
+      <c r="K21" t="s">
         <v>16</v>
       </c>
-      <c r="C21" t="s">
+      <c r="L21" t="s">
         <v>62</v>
       </c>
-      <c r="D21" t="s">
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" t="s">
+        <v>68</v>
+      </c>
+      <c r="F22" t="s">
         <v>63</v>
       </c>
-      <c r="E21" t="s">
-        <v>64</v>
-      </c>
-      <c r="F21" t="s">
+      <c r="G22" t="s">
         <v>65</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H22" t="s">
         <v>66</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I22" t="s">
         <v>67</v>
       </c>
-      <c r="I21" t="s">
-        <v>68</v>
-      </c>
-      <c r="J21" t="s">
-        <v>19</v>
-      </c>
-      <c r="K21" t="s">
-        <v>17</v>
-      </c>
-      <c r="L21" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" t="s">
-        <v>70</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="J22" t="s">
+        <v>72</v>
+      </c>
+      <c r="K22" t="s">
+        <v>73</v>
+      </c>
+      <c r="L22" t="s">
         <v>71</v>
       </c>
-      <c r="E22" t="s">
-        <v>72</v>
-      </c>
-      <c r="F22" t="s">
-        <v>96</v>
-      </c>
-      <c r="G22" t="s">
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H22" t="s">
+      <c r="K23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="I22" t="s">
-        <v>76</v>
-      </c>
-      <c r="J22" t="s">
-        <v>20</v>
-      </c>
-      <c r="K22" t="s">
-        <v>18</v>
-      </c>
-      <c r="L22" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B23" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" t="s">
-        <v>94</v>
-      </c>
-      <c r="D23" t="s">
-        <v>90</v>
-      </c>
-      <c r="E23" t="s">
-        <v>89</v>
-      </c>
-      <c r="F23" t="s">
-        <v>95</v>
-      </c>
-      <c r="G23" t="s">
-        <v>92</v>
-      </c>
-      <c r="H23" t="s">
-        <v>88</v>
-      </c>
-      <c r="I23" t="s">
-        <v>93</v>
-      </c>
-      <c r="J23" t="s">
-        <v>27</v>
-      </c>
-      <c r="K23" t="s">
-        <v>27</v>
-      </c>
-      <c r="L23" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B24" t="s">
-        <v>81</v>
-      </c>
-      <c r="C24" t="s">
-        <v>77</v>
-      </c>
-      <c r="D24" t="s">
-        <v>82</v>
-      </c>
-      <c r="E24" t="s">
-        <v>81</v>
-      </c>
-      <c r="F24" t="s">
-        <v>73</v>
-      </c>
-      <c r="G24" t="s">
-        <v>78</v>
-      </c>
-      <c r="H24" t="s">
-        <v>79</v>
-      </c>
-      <c r="I24" t="s">
-        <v>80</v>
-      </c>
-      <c r="J24" t="s">
-        <v>85</v>
-      </c>
-      <c r="K24" t="s">
-        <v>86</v>
-      </c>
-      <c r="L24" t="s">
-        <v>84</v>
-      </c>
+      <c r="C24" t="b">
+        <v>1</v>
+      </c>
+      <c r="J24" t="b">
+        <v>1</v>
+      </c>
+      <c r="K24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>